<commit_message>
Null checking added. Won't crash when encountering blank rows within data anymore.
</commit_message>
<xml_diff>
--- a/DewaltHangerCalculator/HANGERS LEVEL 2.xlsx
+++ b/DewaltHangerCalculator/HANGERS LEVEL 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsahli\source\repos\DewaltHangerCalculator\DewaltHangerCalculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795FD3B8-F72E-4779-9225-991F0DE89EEE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945E1878-929B-4E81-9CAE-8A63B6415ECF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31980" yWindow="660" windowWidth="21090" windowHeight="13485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HANGERS LEVEL 2" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="51">
   <si>
     <t>CONDUIT RACK HANGER SCHEDULE</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>CN-41</t>
+  </si>
+  <si>
+    <t>FOO BAR</t>
   </si>
 </sst>
 </file>
@@ -1010,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G93"/>
+  <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94:XFD94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3125,6 +3128,11 @@
         <v>14</v>
       </c>
     </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>